<commit_message>
Correct the Stores data
</commit_message>
<xml_diff>
--- a/DataWarehouse/tunisian_data/Tunisian_Data.xlsx
+++ b/DataWarehouse/tunisian_data/Tunisian_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b04d825435d036ce/Documents/DataWarehouse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b04d825435d036ce/Documents/DataWarehouse/DataWarehouse/tunisian_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_71DCB3D93E7877C43F2DF11FD01580A328A461B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB0EB735-E88A-4E27-8C52-B696E10C0206}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_71DCB3D93E7877C43F2DF11FD01580A328A461B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BDD6778-5EE0-4FDE-AD5C-038F3F0A33F4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -1843,6 +1843,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2132,7 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0"/>
+    <sheetView topLeftCell="A324" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12938,9 +12942,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>